<commit_message>
Commit Test Automation V2
</commit_message>
<xml_diff>
--- a/Autothon/extentreport/autothon_TestAutomation.xlsx
+++ b/Autothon/extentreport/autothon_TestAutomation.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Autothon\TestCasesCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A41A79-202B-4A0F-8EA7-F45429AD67B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2E3E1E4B-EB8B-40CA-8174-2FC0CCF0351B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="MoieRentalService_Login" sheetId="3" r:id="rId1"/>
-    <sheet name="Add Movie Description" sheetId="5" r:id="rId2"/>
-    <sheet name="TestCases_MovieRentalServiceLog" sheetId="4" r:id="rId3"/>
+    <sheet name="MoieRentalService_Login" r:id="rId1" sheetId="3"/>
+    <sheet name="Add Movie Description" r:id="rId2" sheetId="5"/>
+    <sheet name="TestCases_MovieRentalService" r:id="rId3" sheetId="4"/>
+    <sheet name="TestCases_ParallelExecution" r:id="rId4" sheetId="6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -107,9 +108,6 @@
     <t>Drama</t>
   </si>
   <si>
-    <t xml:space="preserve">Autothon </t>
-  </si>
-  <si>
     <t>Nagarro</t>
   </si>
   <si>
@@ -132,12 +130,25 @@
   </si>
   <si>
     <t>user should be able to Login</t>
+  </si>
+  <si>
+    <t>Autothon  begins shortly</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>TC01_parallelExecution</t>
+  </si>
+  <si>
+    <t>Two parallel browser sessions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +185,36 @@
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,33 +243,37 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -245,10 +290,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -283,7 +328,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -318,7 +363,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -412,21 +457,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -443,7 +488,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -495,15 +540,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA34AA8-AE65-4E63-A24F-10EFF11301ED}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA34AA8-AE65-4E63-A24F-10EFF11301ED}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -511,9 +556,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -550,23 +595,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670E4616-83F4-41E7-B3F7-6EC69535418E}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670E4616-83F4-41E7-B3F7-6EC69535418E}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="32.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -591,13 +637,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -611,27 +657,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{ACD91764-E60B-4883-99B2-A3E36072F2E9}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{ACD91764-E60B-4883-99B2-A3E36072F2E9}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9491F68E-078D-4EAA-9049-41B2312C8643}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9491F68E-078D-4EAA-9049-41B2312C8643}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="49.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.89453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,9 +704,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -671,37 +718,105 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A10B823-4683-4E3C-B165-0B094C3FAD89}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>